<commit_message>
Update refugee spreadsheet to 9/24 data
</commit_message>
<xml_diff>
--- a/refugees_2015.xlsx
+++ b/refugees_2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14660" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="200" windowWidth="25360" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Bracket" sheetId="3" r:id="rId1"/>
@@ -71,7 +71,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Through 9/22</t>
+Through 9/24</t>
         </r>
       </text>
     </comment>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
   <si>
     <t>Sea arrivals of refugees and migrants to Europe:</t>
   </si>
@@ -263,9 +263,6 @@
     <t>Alternatively, bracket and gut check</t>
   </si>
   <si>
-    <t>Target</t>
-  </si>
-  <si>
     <t>per week</t>
   </si>
   <si>
@@ -311,10 +308,28 @@
     <t>Most recent daily rate:</t>
   </si>
   <si>
-    <t>9/20-9/22</t>
-  </si>
-  <si>
-    <t>9/1-9/20</t>
+    <t>9/22-9/24</t>
+  </si>
+  <si>
+    <t>Put previous update here</t>
+  </si>
+  <si>
+    <t>9/20-9/24</t>
+  </si>
+  <si>
+    <t>Projections based on constant current rate</t>
+  </si>
+  <si>
+    <t>per day</t>
+  </si>
+  <si>
+    <t>Days left</t>
+  </si>
+  <si>
+    <t>Total for year</t>
+  </si>
+  <si>
+    <t>Remaining</t>
   </si>
 </sst>
 </file>
@@ -326,7 +341,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -385,6 +400,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -394,7 +416,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -426,8 +448,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFFF0000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FFFF0000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFFF0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFFF0000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -442,8 +490,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -480,20 +536,32 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="22">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -506,16 +574,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>10160</xdr:rowOff>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>518160</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:rowOff>81280</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -524,8 +592,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3779520" y="396240"/>
-          <a:ext cx="2682240" cy="822960"/>
+          <a:off x="4876800" y="640080"/>
+          <a:ext cx="2682240" cy="833120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -565,19 +633,19 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t> month </a:t>
+            <a:t> month, per week, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>and</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> per day </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>and </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>per week </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t>columns give average rate that would need to see (Italy+Greece+others) for remaining part of 2015 to achieve the corresponding target.</a:t>
+            <a:t>columns give average rate that would need to see (Italy+Greece+others) for remaining part of 2015 to end up the corresponding total.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -1059,10 +1127,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1071,131 +1139,159 @@
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1">
+    <row r="2" spans="1:12" ht="16" thickBot="1">
       <c r="A2" s="1"/>
       <c r="B2" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" thickTop="1" thickBot="1">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="17" thickTop="1" thickBot="1">
       <c r="B3" s="17">
-        <v>487497</v>
+        <v>499826</v>
       </c>
       <c r="C3" s="19">
-        <v>42269</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="16" thickTop="1">
+        <v>42271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="16" thickTop="1">
       <c r="A4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>560000</v>
       </c>
       <c r="B5">
         <f>A5-B3</f>
-        <v>72503</v>
+        <v>60174</v>
       </c>
       <c r="C5" s="5">
         <f>B5/B11</f>
-        <v>22564.709183673469</v>
+        <v>19117.78125</v>
       </c>
       <c r="D5" s="5">
         <f>B5/B10</f>
-        <v>5178.7857142857147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>4387.6875</v>
+      </c>
+      <c r="E5" s="5">
+        <f>B5/B12</f>
+        <v>626.8125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>710000</v>
       </c>
       <c r="B6">
         <f>A6-B3</f>
-        <v>222503</v>
+        <v>210174</v>
       </c>
       <c r="C6" s="5">
         <f>B6/B11</f>
-        <v>69248.382653061228</v>
+        <v>66774.03125</v>
       </c>
       <c r="D6" s="5">
         <f>B6/B10</f>
-        <v>15893.071428571429</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>15325.1875</v>
+      </c>
+      <c r="E6" s="5">
+        <f>B6/B12</f>
+        <v>2189.3125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>1000000</v>
       </c>
       <c r="B7">
         <f>A7-B3</f>
-        <v>512503</v>
+        <v>500174</v>
       </c>
       <c r="C7" s="5">
         <f>B7/B11</f>
-        <v>159503.48469387754</v>
+        <v>158909.44791666666</v>
       </c>
       <c r="D7" s="5">
         <f>B7/B10</f>
-        <v>36607.357142857145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>36471.020833333336</v>
+      </c>
+      <c r="E7" s="25">
+        <f>B7/B12</f>
+        <v>5210.145833333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="16">
         <v>42369</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="4">
         <f>DAYS360(C3,B9,1)/7</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>13.714285714285714</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="4">
         <f>DAYS360(C3,B9,1)/30.5</f>
-        <v>3.2131147540983607</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>3.1475409836065573</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="4">
+        <f>DAYS360(C3,B9,1)</f>
+        <v>96</v>
+      </c>
+      <c r="L12">
+        <f>0.154-0.136</f>
+        <v>1.7999999999999988E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="16" thickBot="1"/>
-    <row r="15" spans="1:4" s="20" customFormat="1" ht="16" thickTop="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="16" thickBot="1"/>
+    <row r="15" spans="1:12" s="20" customFormat="1" ht="16" thickTop="1">
       <c r="B15" s="21"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1204,7 +1300,7 @@
       </c>
       <c r="B18" s="5">
         <f>Italy!G16</f>
-        <v>152634.57342475199</v>
+        <v>147707.78733672961</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1213,7 +1309,7 @@
       </c>
       <c r="B19" s="5">
         <f>Greece!G16</f>
-        <v>687381.1255701636</v>
+        <v>702182.34156157763</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1222,7 +1318,7 @@
       </c>
       <c r="B20" s="5">
         <f>SUM(B18:B19)</f>
-        <v>840015.69899491558</v>
+        <v>849890.12889830722</v>
       </c>
     </row>
   </sheetData>
@@ -1239,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView showRuler="0" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1250,12 +1346,12 @@
     <col min="4" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" ht="42">
+    <row r="2" spans="1:10" s="8" customFormat="1" ht="56">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
@@ -1271,8 +1367,11 @@
       <c r="G2" s="9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1283,7 +1382,7 @@
         <v>1690</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1294,7 +1393,7 @@
         <v>2945</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1305,7 +1404,7 @@
         <v>7634</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1316,7 +1415,7 @@
         <v>13133</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1327,7 +1426,7 @@
         <v>18444</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1338,7 +1437,7 @@
         <v>30717</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1349,7 +1448,7 @@
         <v>51951</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16" thickBot="1">
+    <row r="10" spans="1:10" ht="16" thickBot="1">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1364,7 +1463,7 @@
         <v>0.90448081566943928</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="17" thickTop="1" thickBot="1">
+    <row r="11" spans="1:10" ht="17" thickTop="1" thickBot="1">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1372,7 +1471,7 @@
         <v>7454</v>
       </c>
       <c r="C11" s="17">
-        <v>122708</v>
+        <v>134037</v>
       </c>
       <c r="D11" s="16">
         <v>42277</v>
@@ -1383,10 +1482,14 @@
       </c>
       <c r="G11" s="5">
         <f>DAYS360(Bracket!$C$3,D11,1)*$B$19</f>
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="16" thickTop="1">
+        <v>33987</v>
+      </c>
+      <c r="H11" s="5">
+        <f>DAYS360(Bracket!$C$3,D11,1)*$B$19</f>
+        <v>33987</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="16" thickTop="1">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1402,10 +1505,17 @@
       </c>
       <c r="G12" s="5">
         <f>(C11+G11)*E12</f>
-        <v>162227.77783740274</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>167528.08800643947</v>
+      </c>
+      <c r="H12" s="5">
+        <f>$B$19*31</f>
+        <v>175599.5</v>
+      </c>
+      <c r="J12" s="16">
+        <v>42278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1421,10 +1531,17 @@
       </c>
       <c r="G13" s="5">
         <f>(C11+G11)*E13</f>
-        <v>83209.40381003487</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>85928.023611483761</v>
+      </c>
+      <c r="H13" s="5">
+        <f>$B$19*30</f>
+        <v>169935</v>
+      </c>
+      <c r="J13" s="16">
+        <v>42309</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1440,19 +1557,30 @@
       </c>
       <c r="G14" s="5">
         <f>(C11+G11)*E14</f>
-        <v>44878.943922726052</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>46345.229943654413</v>
+      </c>
+      <c r="H14" s="5">
+        <f>$B$19*31</f>
+        <v>175599.5</v>
+      </c>
+      <c r="J14" s="16">
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="F15" s="10" t="s">
         <v>24</v>
       </c>
       <c r="G15" s="5">
-        <f>AVERAGE(G11:G14)</f>
-        <v>82579.031392540914</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <f>AVERAGE(G12:G14)</f>
+        <v>99933.780520525877</v>
+      </c>
+      <c r="H15" s="5">
+        <f>AVERAGE(H12:H14)</f>
+        <v>173711.33333333334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1462,29 +1590,46 @@
       </c>
       <c r="C16">
         <f>SUM(C3:C14)</f>
-        <v>357065</v>
+        <v>368394</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="5">
         <f>SUM(C3:C11)+SUM(G11:G14)</f>
-        <v>687381.1255701636</v>
+        <v>702182.34156157763</v>
+      </c>
+      <c r="H16" s="5">
+        <f>SUM(C3:C11)+SUM(H11:H14)</f>
+        <v>923515</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16" thickBot="1"/>
     <row r="19" spans="1:3" ht="30" thickTop="1" thickBot="1">
       <c r="A19" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="18">
+        <f>(C11-B21)/2</f>
+        <v>5664.5</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="17">
-        <v>5000</v>
-      </c>
-      <c r="C19" s="6" t="s">
+    </row>
+    <row r="20" spans="1:3" ht="17" thickTop="1" thickBot="1"/>
+    <row r="21" spans="1:3" ht="17" thickTop="1" thickBot="1">
+      <c r="A21" s="22">
+        <v>42269</v>
+      </c>
+      <c r="B21" s="23">
+        <v>122708</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="16" thickTop="1"/>
+    <row r="22" spans="1:3" ht="16" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1499,10 +1644,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1636,7 +1781,7 @@
         <v>26107</v>
       </c>
       <c r="C11" s="17">
-        <v>11851</v>
+        <v>12851</v>
       </c>
       <c r="D11" s="15">
         <v>42277</v>
@@ -1647,7 +1792,7 @@
       </c>
       <c r="G11" s="5">
         <f>DAYS360(Bracket!$C$3,Italy!D11,1)*$B$20</f>
-        <v>4740.3999999999996</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="16" thickTop="1">
@@ -1663,7 +1808,7 @@
       </c>
       <c r="G12" s="5">
         <f>E12*(C11+G11)</f>
-        <v>9708.7684452445701</v>
+        <v>8397.7564254797562</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1679,7 +1824,7 @@
       </c>
       <c r="G13" s="5">
         <f>E13*(C11+G11)</f>
-        <v>5907.1154479641482</v>
+        <v>5109.4551269774383</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1695,7 +1840,7 @@
       </c>
       <c r="G14" s="5">
         <f>E14*(C11+G11)</f>
-        <v>4278.2895315432643</v>
+        <v>3700.575784272417</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1708,27 +1853,39 @@
       </c>
       <c r="C16">
         <f>SUM(C3:C14)</f>
-        <v>128000</v>
+        <v>129000</v>
       </c>
       <c r="G16">
         <f>SUM(C3:C11)+SUM(G11:G14)</f>
-        <v>152634.57342475199</v>
+        <v>147707.78733672961</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16" thickBot="1"/>
     <row r="20" spans="1:3" ht="30" thickTop="1" thickBot="1">
       <c r="A20" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="18">
-        <f>11851/20</f>
-        <v>592.54999999999995</v>
+        <f>(C11-B22)/4</f>
+        <v>250</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="16" thickTop="1"/>
+    <row r="21" spans="1:3" ht="17" thickTop="1" thickBot="1"/>
+    <row r="22" spans="1:3" ht="17" thickTop="1" thickBot="1">
+      <c r="A22" s="24">
+        <v>42267</v>
+      </c>
+      <c r="B22" s="23">
+        <v>11851</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1773,10 +1930,10 @@
         <v>14</v>
       </c>
       <c r="E2" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>44</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1918,7 +2075,7 @@
         <v>40000</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2013,7 +2170,7 @@
         <v>532972</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2031,7 +2188,7 @@
         <v>596178.73242461076</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2040,7 +2197,7 @@
         <v>624021.51000372076</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2049,7 +2206,7 @@
         <v>626795.84011901962</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2058,7 +2215,7 @@
         <v>705220.05917318841</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update refugee spreadsheet to 9/27
</commit_message>
<xml_diff>
--- a/refugees_2015.xlsx
+++ b/refugees_2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="200" windowWidth="25360" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="200" windowWidth="25360" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Bracket" sheetId="3" r:id="rId1"/>
@@ -71,7 +71,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Through 9/24</t>
+Through 9/27</t>
         </r>
       </text>
     </comment>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t>Sea arrivals of refugees and migrants to Europe:</t>
   </si>
@@ -308,15 +308,9 @@
     <t>Most recent daily rate:</t>
   </si>
   <si>
-    <t>9/22-9/24</t>
-  </si>
-  <si>
     <t>Put previous update here</t>
   </si>
   <si>
-    <t>9/20-9/24</t>
-  </si>
-  <si>
     <t>Projections based on constant current rate</t>
   </si>
   <si>
@@ -330,6 +324,21 @@
   </si>
   <si>
     <t>Remaining</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>5 New in Malta</t>
+  </si>
+  <si>
+    <t>9/24-9/27</t>
+  </si>
+  <si>
+    <t>9/24-9/28</t>
+  </si>
+  <si>
+    <t>average arrivals in last 4 months of year, 2014</t>
   </si>
 </sst>
 </file>
@@ -416,7 +425,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -474,8 +483,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -498,8 +516,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -540,8 +562,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -552,6 +576,8 @@
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -562,6 +588,8 @@
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1127,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1139,12 +1167,12 @@
     <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16" thickBot="1">
+    <row r="2" spans="1:5" ht="16" thickBot="1">
       <c r="A2" s="1"/>
       <c r="B2" s="6" t="s">
         <v>18</v>
@@ -1153,20 +1181,20 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17" thickTop="1" thickBot="1">
+    <row r="3" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="B3" s="17">
-        <v>499826</v>
+        <v>520957</v>
       </c>
       <c r="C3" s="19">
-        <v>42271</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="16" thickTop="1">
+        <v>42274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="16" thickTop="1">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>34</v>
@@ -1175,73 +1203,73 @@
         <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>560000</v>
       </c>
       <c r="B5">
         <f>A5-B3</f>
-        <v>60174</v>
+        <v>39043</v>
       </c>
       <c r="C5" s="5">
         <f>B5/B11</f>
-        <v>19117.78125</v>
+        <v>12804.424731182797</v>
       </c>
       <c r="D5" s="5">
         <f>B5/B10</f>
-        <v>4387.6875</v>
+        <v>2938.7204301075267</v>
       </c>
       <c r="E5" s="5">
         <f>B5/B12</f>
-        <v>626.8125</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>419.81720430107526</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>710000</v>
       </c>
       <c r="B6">
         <f>A6-B3</f>
-        <v>210174</v>
+        <v>189043</v>
       </c>
       <c r="C6" s="5">
         <f>B6/B11</f>
-        <v>66774.03125</v>
+        <v>61997.973118279573</v>
       </c>
       <c r="D6" s="5">
         <f>B6/B10</f>
-        <v>15325.1875</v>
+        <v>14229.043010752688</v>
       </c>
       <c r="E6" s="5">
         <f>B6/B12</f>
-        <v>2189.3125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>2032.7204301075269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>1000000</v>
       </c>
       <c r="B7">
         <f>A7-B3</f>
-        <v>500174</v>
+        <v>479043</v>
       </c>
       <c r="C7" s="5">
         <f>B7/B11</f>
-        <v>158909.44791666666</v>
+        <v>157105.5</v>
       </c>
       <c r="D7" s="5">
         <f>B7/B10</f>
-        <v>36471.020833333336</v>
+        <v>36057</v>
       </c>
       <c r="E7" s="25">
         <f>B7/B12</f>
-        <v>5210.145833333333</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>5151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>37</v>
       </c>
@@ -1249,44 +1277,40 @@
         <v>42369</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="4">
         <f>DAYS360(C3,B9,1)/7</f>
-        <v>13.714285714285714</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>13.285714285714286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="4">
         <f>DAYS360(C3,B9,1)/30.5</f>
-        <v>3.1475409836065573</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>3.0491803278688523</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B12" s="4">
         <f>DAYS360(C3,B9,1)</f>
-        <v>96</v>
-      </c>
-      <c r="L12">
-        <f>0.154-0.136</f>
-        <v>1.7999999999999988E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="16" thickBot="1"/>
-    <row r="15" spans="1:12" s="20" customFormat="1" ht="16" thickTop="1">
+    <row r="14" spans="1:5" ht="16" thickBot="1"/>
+    <row r="15" spans="1:5" s="20" customFormat="1" ht="16" thickTop="1">
       <c r="B15" s="21"/>
     </row>
     <row r="17" spans="1:2">
@@ -1300,7 +1324,7 @@
       </c>
       <c r="B18" s="5">
         <f>Italy!G16</f>
-        <v>147707.78733672961</v>
+        <v>152105.91810625503</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1309,7 +1333,7 @@
       </c>
       <c r="B19" s="5">
         <f>Greece!G16</f>
-        <v>702182.34156157763</v>
+        <v>714057.28253286821</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1318,7 +1342,21 @@
       </c>
       <c r="B20" s="5">
         <f>SUM(B18:B19)</f>
-        <v>849890.12889830722</v>
+        <v>866163.20063912321</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" s="26" customFormat="1" ht="16" thickBot="1"/>
+    <row r="23" spans="1:2" ht="16" thickTop="1">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="15">
+        <v>42274</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1337,8 +1375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView showRuler="0" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1368,7 +1406,7 @@
         <v>23</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1471,7 +1509,7 @@
         <v>7454</v>
       </c>
       <c r="C11" s="17">
-        <v>134037</v>
+        <v>153163</v>
       </c>
       <c r="D11" s="16">
         <v>42277</v>
@@ -1482,11 +1520,11 @@
       </c>
       <c r="G11" s="5">
         <f>DAYS360(Bracket!$C$3,D11,1)*$B$19</f>
-        <v>33987</v>
+        <v>19126</v>
       </c>
       <c r="H11" s="5">
         <f>DAYS360(Bracket!$C$3,D11,1)*$B$19</f>
-        <v>33987</v>
+        <v>19126</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16" thickTop="1">
@@ -1505,11 +1543,11 @@
       </c>
       <c r="G12" s="5">
         <f>(C11+G11)*E12</f>
-        <v>167528.08800643947</v>
+        <v>171780.50013415614</v>
       </c>
       <c r="H12" s="5">
         <f>$B$19*31</f>
-        <v>175599.5</v>
+        <v>197635.33333333331</v>
       </c>
       <c r="J12" s="16">
         <v>42278</v>
@@ -1531,11 +1569,11 @@
       </c>
       <c r="G13" s="5">
         <f>(C11+G11)*E13</f>
-        <v>85928.023611483761</v>
+        <v>88109.158572578468</v>
       </c>
       <c r="H13" s="5">
         <f>$B$19*30</f>
-        <v>169935</v>
+        <v>191260</v>
       </c>
       <c r="J13" s="16">
         <v>42309</v>
@@ -1557,11 +1595,11 @@
       </c>
       <c r="G14" s="5">
         <f>(C11+G11)*E14</f>
-        <v>46345.229943654413</v>
+        <v>47521.623826133618</v>
       </c>
       <c r="H14" s="5">
         <f>$B$19*31</f>
-        <v>175599.5</v>
+        <v>197635.33333333331</v>
       </c>
       <c r="J14" s="16">
         <v>42339</v>
@@ -1573,11 +1611,11 @@
       </c>
       <c r="G15" s="5">
         <f>AVERAGE(G12:G14)</f>
-        <v>99933.780520525877</v>
+        <v>102470.42751095607</v>
       </c>
       <c r="H15" s="5">
         <f>AVERAGE(H12:H14)</f>
-        <v>173711.33333333334</v>
+        <v>195510.22222222222</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1590,18 +1628,18 @@
       </c>
       <c r="C16">
         <f>SUM(C3:C14)</f>
-        <v>368394</v>
+        <v>387520</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G16" s="5">
         <f>SUM(C3:C11)+SUM(G11:G14)</f>
-        <v>702182.34156157763</v>
+        <v>714057.28253286821</v>
       </c>
       <c r="H16" s="5">
         <f>SUM(C3:C11)+SUM(H11:H14)</f>
-        <v>923515</v>
+        <v>993176.66666666663</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16" thickBot="1"/>
@@ -1610,26 +1648,33 @@
         <v>47</v>
       </c>
       <c r="B19" s="18">
-        <f>(C11-B21)/2</f>
-        <v>5664.5</v>
+        <f>(C11-B21)/3</f>
+        <v>6375.333333333333</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" thickTop="1" thickBot="1"/>
     <row r="21" spans="1:3" ht="17" thickTop="1" thickBot="1">
       <c r="A21" s="22">
+        <v>42271</v>
+      </c>
+      <c r="B21" s="23">
+        <v>134037</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16" thickTop="1">
+      <c r="A22" s="27">
         <v>42269</v>
       </c>
-      <c r="B21" s="23">
+      <c r="B22">
         <v>122708</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="16" thickTop="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1646,8 +1691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView showRuler="0" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1781,7 +1826,7 @@
         <v>26107</v>
       </c>
       <c r="C11" s="17">
-        <v>12851</v>
+        <v>14851</v>
       </c>
       <c r="D11" s="15">
         <v>42277</v>
@@ -1808,7 +1853,7 @@
       </c>
       <c r="G12" s="5">
         <f>E12*(C11+G11)</f>
-        <v>8397.7564254797562</v>
+        <v>9568.093882866664</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1824,7 +1869,7 @@
       </c>
       <c r="G13" s="5">
         <f>E13*(C11+G11)</f>
-        <v>5109.4551269774383</v>
+        <v>5821.5246868655913</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1840,7 +1885,7 @@
       </c>
       <c r="G14" s="5">
         <f>E14*(C11+G11)</f>
-        <v>3700.575784272417</v>
+        <v>4216.2995365227716</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1853,11 +1898,11 @@
       </c>
       <c r="C16">
         <f>SUM(C3:C14)</f>
-        <v>129000</v>
+        <v>131000</v>
       </c>
       <c r="G16">
         <f>SUM(C3:C11)+SUM(G11:G14)</f>
-        <v>147707.78733672961</v>
+        <v>152105.91810625503</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16" thickBot="1"/>
@@ -1867,25 +1912,32 @@
       </c>
       <c r="B20" s="18">
         <f>(C11-B22)/4</f>
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="17" thickTop="1" thickBot="1"/>
     <row r="22" spans="1:3" ht="17" thickTop="1" thickBot="1">
       <c r="A22" s="24">
+        <v>42271</v>
+      </c>
+      <c r="B22" s="23">
+        <v>12851</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16" thickTop="1">
+      <c r="A23" s="16">
         <v>42267</v>
       </c>
-      <c r="B22" s="23">
+      <c r="B23">
         <v>11851</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="16" thickTop="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1900,10 +1952,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1911,12 +1963,12 @@
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45">
+    <row r="2" spans="1:13" ht="45">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1936,7 +1988,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1951,7 +2003,7 @@
         <v>1.6960244648318044</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1966,7 +2018,7 @@
         <v>1.6807049668116274</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1981,7 +2033,7 @@
         <v>1.3983248661265961</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1996,7 +2048,7 @@
         <v>1.7233083586981972</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -2011,7 +2063,7 @@
         <v>2.4127623744511939</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -2026,7 +2078,7 @@
         <v>2.0589222379009193</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -2041,7 +2093,7 @@
         <v>2.6669610995300852</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -2056,7 +2108,7 @@
         <v>3.9081486349244279</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2064,21 +2116,21 @@
         <v>33944</v>
       </c>
       <c r="C11">
-        <v>134559</v>
+        <v>168019</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>3.9641468300730613</v>
+        <v>4.9498880509073766</v>
       </c>
       <c r="F11">
-        <f>8*5000</f>
-        <v>40000</v>
+        <f>3*5000</f>
+        <v>15000</v>
       </c>
       <c r="G11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -2091,10 +2143,16 @@
       </c>
       <c r="F12" s="5">
         <f>(F11+C11)*E12</f>
-        <v>118535.96953806269</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>124280.81398774452</v>
+      </c>
+      <c r="K12">
+        <v>33944</v>
+      </c>
+      <c r="L12" s="15">
+        <v>41883</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -2107,10 +2165,13 @@
       </c>
       <c r="F13" s="5">
         <f>(F11+C11)*E13</f>
-        <v>68488.591857176521</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>71807.890702333258</v>
+      </c>
+      <c r="K13">
+        <v>23050</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -2123,10 +2184,21 @@
       </c>
       <c r="F14" s="5">
         <f>(F11+C11)*E14</f>
-        <v>46833.278723780342</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>49103.053057977842</v>
+      </c>
+      <c r="K14">
+        <v>13318</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="K15">
+        <v>9107</v>
+      </c>
+      <c r="L15" s="15">
+        <v>42004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -2136,17 +2208,28 @@
       </c>
       <c r="C16" s="3">
         <f>SUM(C3:C14)</f>
-        <v>487497</v>
+        <v>520957</v>
       </c>
       <c r="D16" s="2">
         <f>AVERAGE(D3:D11)</f>
-        <v>2.3899226481497684</v>
+        <v>2.499449450464692</v>
+      </c>
+      <c r="K16">
+        <f>SUM(K12:K15)</f>
+        <v>79419</v>
+      </c>
+      <c r="L16" s="5">
+        <f>K16/(DAYS360(L12,L15,1))</f>
+        <v>667.38655462184875</v>
+      </c>
+      <c r="M16" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="D17" s="2">
         <f>AVERAGE(D7:D11)</f>
-        <v>3.0021882353759373</v>
+        <v>3.1993364795428008</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2167,7 +2250,7 @@
     <row r="22" spans="1:4">
       <c r="B22">
         <f>C16+B18</f>
-        <v>532972</v>
+        <v>566432</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>39</v>
@@ -2176,7 +2259,7 @@
     <row r="23" spans="1:4">
       <c r="B23" s="5">
         <f>C16+2.5*B18</f>
-        <v>601184.5</v>
+        <v>634644.5</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>16</v>
@@ -2185,7 +2268,7 @@
     <row r="24" spans="1:4">
       <c r="B24" s="5">
         <f>C16+B18*D16</f>
-        <v>596178.73242461076</v>
+        <v>634619.46375988191</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>40</v>
@@ -2194,7 +2277,7 @@
     <row r="25" spans="1:4">
       <c r="B25" s="5">
         <f>C16+B18*D17</f>
-        <v>624021.51000372076</v>
+        <v>666446.82640720881</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>41</v>
@@ -2203,7 +2286,7 @@
     <row r="26" spans="1:4">
       <c r="B26" s="5">
         <f>SUM(C3:C10)+SUM(F11:F14)</f>
-        <v>626795.84011901962</v>
+        <v>613129.75774805562</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>42</v>
@@ -2212,7 +2295,7 @@
     <row r="27" spans="1:4">
       <c r="B27" s="5">
         <f>C16+B18*D10+F11</f>
-        <v>705220.05917318841</v>
+        <v>713680.05917318841</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Update refugee files, add ordered categorical scoring tool
</commit_message>
<xml_diff>
--- a/refugees_2015.xlsx
+++ b/refugees_2015.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="200" windowWidth="25360" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="14160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Bracket" sheetId="3" r:id="rId1"/>
@@ -71,7 +71,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Through 9/27</t>
+Through 9/27 (unclear if this is correct or editor forgot to update. Value on website 10/2)</t>
         </r>
       </text>
     </comment>
@@ -332,13 +332,13 @@
     <t>5 New in Malta</t>
   </si>
   <si>
-    <t>9/24-9/27</t>
-  </si>
-  <si>
     <t>9/24-9/28</t>
   </si>
   <si>
     <t>average arrivals in last 4 months of year, 2014</t>
+  </si>
+  <si>
+    <t>9/28-9/30</t>
   </si>
 </sst>
 </file>
@@ -493,9 +493,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="26">
+  <cellStyleXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -565,7 +567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="26">
+  <cellStyles count="28">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -578,6 +580,7 @@
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -590,11 +593,17 @@
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF99E48F"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -756,10 +765,154 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>172720</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>162560</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3322320" y="121920"/>
+          <a:ext cx="3190240" cy="436880"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="CCFFCC"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Appropriate</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> date for this update unclear. Values as of 10/2 - probably correct through 9/30</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>386080</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>10160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>467360</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>172720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2854960" y="3850640"/>
+          <a:ext cx="2936240" cy="751840"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="CCFFCC"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+              <a:alpha val="89000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>10/2</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>  Website updated but Greece figures say "as of Sep 27" still. Not sure if figures are revised for 9/27 or ar through end of month.  Sum of months doesn't match website now</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1155,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1183,10 +1336,10 @@
     </row>
     <row r="3" spans="1:5" ht="17" thickTop="1" thickBot="1">
       <c r="B3" s="17">
-        <v>520957</v>
+        <v>529937</v>
       </c>
       <c r="C3" s="19">
-        <v>42274</v>
+        <v>42277</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" thickTop="1">
@@ -1212,19 +1365,19 @@
       </c>
       <c r="B5">
         <f>A5-B3</f>
-        <v>39043</v>
+        <v>30063</v>
       </c>
       <c r="C5" s="5">
         <f>B5/B11</f>
-        <v>12804.424731182797</v>
+        <v>10188.016666666666</v>
       </c>
       <c r="D5" s="5">
         <f>B5/B10</f>
-        <v>2938.7204301075267</v>
+        <v>2338.2333333333331</v>
       </c>
       <c r="E5" s="5">
         <f>B5/B12</f>
-        <v>419.81720430107526</v>
+        <v>334.03333333333336</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1233,19 +1386,19 @@
       </c>
       <c r="B6">
         <f>A6-B3</f>
-        <v>189043</v>
+        <v>180063</v>
       </c>
       <c r="C6" s="5">
         <f>B6/B11</f>
-        <v>61997.973118279573</v>
+        <v>61021.35</v>
       </c>
       <c r="D6" s="5">
         <f>B6/B10</f>
-        <v>14229.043010752688</v>
+        <v>14004.9</v>
       </c>
       <c r="E6" s="5">
         <f>B6/B12</f>
-        <v>2032.7204301075269</v>
+        <v>2000.7</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1254,19 +1407,19 @@
       </c>
       <c r="B7">
         <f>A7-B3</f>
-        <v>479043</v>
+        <v>470063</v>
       </c>
       <c r="C7" s="5">
         <f>B7/B11</f>
-        <v>157105.5</v>
+        <v>159299.12777777776</v>
       </c>
       <c r="D7" s="5">
         <f>B7/B10</f>
-        <v>36057</v>
+        <v>36560.455555555556</v>
       </c>
       <c r="E7" s="25">
         <f>B7/B12</f>
-        <v>5151</v>
+        <v>5222.9222222222224</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1283,7 +1436,7 @@
       </c>
       <c r="B10" s="4">
         <f>DAYS360(C3,B9,1)/7</f>
-        <v>13.285714285714286</v>
+        <v>12.857142857142858</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1292,7 +1445,7 @@
       </c>
       <c r="B11" s="4">
         <f>DAYS360(C3,B9,1)/30.5</f>
-        <v>3.0491803278688523</v>
+        <v>2.9508196721311477</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1301,7 +1454,7 @@
       </c>
       <c r="B12" s="4">
         <f>DAYS360(C3,B9,1)</f>
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1324,7 +1477,7 @@
       </c>
       <c r="B18" s="5">
         <f>Italy!G16</f>
-        <v>152105.91810625503</v>
+        <v>148807.32002911097</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1333,7 +1486,7 @@
       </c>
       <c r="B19" s="5">
         <f>Greece!G16</f>
-        <v>714057.28253286821</v>
+        <v>683516.54923530994</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1342,7 +1495,7 @@
       </c>
       <c r="B20" s="5">
         <f>SUM(B18:B19)</f>
-        <v>866163.20063912321</v>
+        <v>832323.86926442094</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="26" customFormat="1" ht="16" thickBot="1"/>
@@ -1358,6 +1511,9 @@
       <c r="B24" t="s">
         <v>55</v>
       </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1373,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView showRuler="0" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1509,7 +1665,7 @@
         <v>7454</v>
       </c>
       <c r="C11" s="17">
-        <v>153163</v>
+        <v>161320</v>
       </c>
       <c r="D11" s="16">
         <v>42277</v>
@@ -1520,11 +1676,11 @@
       </c>
       <c r="G11" s="5">
         <f>DAYS360(Bracket!$C$3,D11,1)*$B$19</f>
-        <v>19126</v>
+        <v>0</v>
       </c>
       <c r="H11" s="5">
         <f>DAYS360(Bracket!$C$3,D11,1)*$B$19</f>
-        <v>19126</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="16" thickTop="1">
@@ -1543,11 +1699,11 @@
       </c>
       <c r="G12" s="5">
         <f>(C11+G11)*E12</f>
-        <v>171780.50013415614</v>
+        <v>160843.87442983632</v>
       </c>
       <c r="H12" s="5">
         <f>$B$19*31</f>
-        <v>197635.33333333331</v>
+        <v>84289</v>
       </c>
       <c r="J12" s="16">
         <v>42278</v>
@@ -1569,11 +1725,11 @@
       </c>
       <c r="G13" s="5">
         <f>(C11+G11)*E13</f>
-        <v>88109.158572578468</v>
+        <v>82499.576066541442</v>
       </c>
       <c r="H13" s="5">
         <f>$B$19*30</f>
-        <v>191260</v>
+        <v>81570</v>
       </c>
       <c r="J13" s="16">
         <v>42309</v>
@@ -1595,11 +1751,11 @@
       </c>
       <c r="G14" s="5">
         <f>(C11+G11)*E14</f>
-        <v>47521.623826133618</v>
+        <v>44496.098738932116</v>
       </c>
       <c r="H14" s="5">
         <f>$B$19*31</f>
-        <v>197635.33333333331</v>
+        <v>84289</v>
       </c>
       <c r="J14" s="16">
         <v>42339</v>
@@ -1611,11 +1767,11 @@
       </c>
       <c r="G15" s="5">
         <f>AVERAGE(G12:G14)</f>
-        <v>102470.42751095607</v>
+        <v>95946.516411769961</v>
       </c>
       <c r="H15" s="5">
         <f>AVERAGE(H12:H14)</f>
-        <v>195510.22222222222</v>
+        <v>83382.666666666672</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1628,18 +1784,18 @@
       </c>
       <c r="C16">
         <f>SUM(C3:C14)</f>
-        <v>387520</v>
+        <v>395677</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>25</v>
       </c>
       <c r="G16" s="5">
         <f>SUM(C3:C11)+SUM(G11:G14)</f>
-        <v>714057.28253286821</v>
+        <v>683516.54923530994</v>
       </c>
       <c r="H16" s="5">
         <f>SUM(C3:C11)+SUM(H11:H14)</f>
-        <v>993176.66666666663</v>
+        <v>645825</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="16" thickBot="1"/>
@@ -1649,19 +1805,19 @@
       </c>
       <c r="B19" s="18">
         <f>(C11-B21)/3</f>
-        <v>6375.333333333333</v>
+        <v>2719</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17" thickTop="1" thickBot="1"/>
     <row r="21" spans="1:3" ht="17" thickTop="1" thickBot="1">
       <c r="A21" s="22">
-        <v>42271</v>
+        <v>42274</v>
       </c>
       <c r="B21" s="23">
-        <v>134037</v>
+        <v>153163</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>48</v>
@@ -1669,16 +1825,25 @@
     </row>
     <row r="22" spans="1:3" ht="16" thickTop="1">
       <c r="A22" s="27">
+        <v>42271</v>
+      </c>
+      <c r="B22">
+        <v>134037</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
         <v>42269</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>122708</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>
@@ -1837,7 +2002,7 @@
       </c>
       <c r="G11" s="5">
         <f>DAYS360(Bracket!$C$3,Italy!D11,1)*$B$20</f>
-        <v>1500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="16" thickTop="1">
@@ -1853,7 +2018,7 @@
       </c>
       <c r="G12" s="5">
         <f>E12*(C11+G11)</f>
-        <v>9568.093882866664</v>
+        <v>8690.3407898264832</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1869,7 +2034,7 @@
       </c>
       <c r="G13" s="5">
         <f>E13*(C11+G11)</f>
-        <v>5821.5246868655913</v>
+        <v>5287.4725169494768</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1885,7 +2050,7 @@
       </c>
       <c r="G14" s="5">
         <f>E14*(C11+G11)</f>
-        <v>4216.2995365227716</v>
+        <v>3829.5067223350056</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1902,7 +2067,7 @@
       </c>
       <c r="G16">
         <f>SUM(C3:C11)+SUM(G11:G14)</f>
-        <v>152105.91810625503</v>
+        <v>148807.32002911097</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="16" thickBot="1"/>
@@ -1915,7 +2080,7 @@
         <v>500</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="17" thickTop="1" thickBot="1"/>
@@ -1954,8 +2119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView showRuler="0" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2116,15 +2281,15 @@
         <v>33944</v>
       </c>
       <c r="C11">
-        <v>168019</v>
+        <v>176176</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>4.9498880509073766</v>
+        <v>5.1901956163092153</v>
       </c>
       <c r="F11">
-        <f>3*5000</f>
-        <v>15000</v>
+        <f>0*5000</f>
+        <v>0</v>
       </c>
       <c r="G11" t="s">
         <v>38</v>
@@ -2143,7 +2308,7 @@
       </c>
       <c r="F12" s="5">
         <f>(F11+C11)*E12</f>
-        <v>124280.81398774452</v>
+        <v>119634.00895592741</v>
       </c>
       <c r="K12">
         <v>33944</v>
@@ -2165,7 +2330,7 @@
       </c>
       <c r="F13" s="5">
         <f>(F11+C11)*E13</f>
-        <v>71807.890702333258</v>
+        <v>69123.025218006122</v>
       </c>
       <c r="K13">
         <v>23050</v>
@@ -2184,7 +2349,7 @@
       </c>
       <c r="F14" s="5">
         <f>(F11+C11)*E14</f>
-        <v>49103.053057977842</v>
+        <v>47267.111477728024</v>
       </c>
       <c r="K14">
         <v>13318</v>
@@ -2208,11 +2373,11 @@
       </c>
       <c r="C16" s="3">
         <f>SUM(C3:C14)</f>
-        <v>520957</v>
+        <v>529114</v>
       </c>
       <c r="D16" s="2">
         <f>AVERAGE(D3:D11)</f>
-        <v>2.499449450464692</v>
+        <v>2.5261502910648961</v>
       </c>
       <c r="K16">
         <f>SUM(K12:K15)</f>
@@ -2223,13 +2388,13 @@
         <v>667.38655462184875</v>
       </c>
       <c r="M16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="D17" s="2">
         <f>AVERAGE(D7:D11)</f>
-        <v>3.1993364795428008</v>
+        <v>3.2473979926231684</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2250,7 +2415,7 @@
     <row r="22" spans="1:4">
       <c r="B22">
         <f>C16+B18</f>
-        <v>566432</v>
+        <v>574589</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>39</v>
@@ -2259,7 +2424,7 @@
     <row r="23" spans="1:4">
       <c r="B23" s="5">
         <f>C16+2.5*B18</f>
-        <v>634644.5</v>
+        <v>642801.5</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>16</v>
@@ -2268,7 +2433,7 @@
     <row r="24" spans="1:4">
       <c r="B24" s="5">
         <f>C16+B18*D16</f>
-        <v>634619.46375988191</v>
+        <v>643990.68448617612</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>40</v>
@@ -2277,7 +2442,7 @@
     <row r="25" spans="1:4">
       <c r="B25" s="5">
         <f>C16+B18*D17</f>
-        <v>666446.82640720881</v>
+        <v>676789.42371453857</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>41</v>
@@ -2286,7 +2451,7 @@
     <row r="26" spans="1:4">
       <c r="B26" s="5">
         <f>SUM(C3:C10)+SUM(F11:F14)</f>
-        <v>613129.75774805562</v>
+        <v>588962.14565166156</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>42</v>
@@ -2295,7 +2460,7 @@
     <row r="27" spans="1:4">
       <c r="B27" s="5">
         <f>C16+B18*D10+F11</f>
-        <v>713680.05917318841</v>
+        <v>706837.05917318841</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>45</v>

</xml_diff>